<commit_message>
Tooltip de botin ordenado y filtrado
</commit_message>
<xml_diff>
--- a/LogBook/Locale/Locale.xlsx
+++ b/LogBook/Locale/Locale.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="152">
   <si>
     <t xml:space="preserve">Delete character data</t>
   </si>
@@ -127,6 +127,12 @@
     <t xml:space="preserve">Mayúsculas + Control</t>
   </si>
   <si>
+    <t xml:space="preserve">Press key to show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulse la tecla para mostrar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Accept</t>
   </si>
   <si>
@@ -337,6 +343,12 @@
     <t xml:space="preserve">Estadísticas</t>
   </si>
   <si>
+    <t xml:space="preserve">Tooltips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mensaje emergente</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maintenance</t>
   </si>
   <si>
@@ -367,10 +379,10 @@
     <t xml:space="preserve">¡Hecho!</t>
   </si>
   <si>
-    <t xml:space="preserve">Tooltips</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mensaje emergente</t>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todos</t>
   </si>
   <si>
     <t xml:space="preserve">Database</t>
@@ -379,28 +391,91 @@
     <t xml:space="preserve">Base de datos</t>
   </si>
   <si>
-    <t xml:space="preserve">Press key to show</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pulse la tecla para mostrar</t>
-  </si>
-  <si>
     <t xml:space="preserve">more</t>
   </si>
   <si>
     <t xml:space="preserve">más</t>
   </si>
   <si>
-    <t xml:space="preserve">Character</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personaje</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Character name.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre del personaje.</t>
+    <t xml:space="preserve">Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Élite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rare elite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raro élite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jefe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World boss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jefe de mundo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pobre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Común</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncommon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poco Común</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legendary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legendario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artifact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artefacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heirloom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reliquia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WoW Token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ficha WoW</t>
   </si>
 </sst>
 </file>
@@ -613,8 +688,8 @@
   </sheetPr>
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D61" activeCellId="0" sqref="D:D"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -937,11 +1012,11 @@
       </c>
       <c r="C20" s="1" t="str">
         <f aca="false">IF(A20="", "", "L["""&amp;A20&amp;"""] = true")</f>
-        <v>L["Accept"] = true</v>
+        <v>L["Press key to show"] = true</v>
       </c>
       <c r="D20" s="1" t="str">
         <f aca="false">IF(A20="", "", "L["""&amp;A20&amp;"""] = """ &amp; B20 &amp; """")</f>
-        <v>L["Accept"] = "Aceptar"</v>
+        <v>L["Press key to show"] = "Pulse la tecla para mostrar"</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,11 +1028,11 @@
       </c>
       <c r="C21" s="1" t="str">
         <f aca="false">IF(A21="", "", "L["""&amp;A21&amp;"""] = true")</f>
-        <v>L["Cancel"] = true</v>
+        <v>L["Accept"] = true</v>
       </c>
       <c r="D21" s="1" t="str">
         <f aca="false">IF(A21="", "", "L["""&amp;A21&amp;"""] = """ &amp; B21 &amp; """")</f>
-        <v>L["Cancel"] = "Cancelar"</v>
+        <v>L["Accept"] = "Aceptar"</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,11 +1044,11 @@
       </c>
       <c r="C22" s="1" t="str">
         <f aca="false">IF(A22="", "", "L["""&amp;A22&amp;"""] = true")</f>
-        <v>L["Module |cffffcc00%s|r loaded"] = true</v>
+        <v>L["Cancel"] = true</v>
       </c>
       <c r="D22" s="1" t="str">
         <f aca="false">IF(A22="", "", "L["""&amp;A22&amp;"""] = """ &amp; B22 &amp; """")</f>
-        <v>L["Module |cffffcc00%s|r loaded"] = "Módulo |cffffcc00%s|r cargado"</v>
+        <v>L["Cancel"] = "Cancelar"</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,11 +1060,11 @@
       </c>
       <c r="C23" s="1" t="str">
         <f aca="false">IF(A23="", "", "L["""&amp;A23&amp;"""] = true")</f>
-        <v>L["LogBook %s initialized"] = true</v>
+        <v>L["Module |cffffcc00%s|r loaded"] = true</v>
       </c>
       <c r="D23" s="1" t="str">
         <f aca="false">IF(A23="", "", "L["""&amp;A23&amp;"""] = """ &amp; B23 &amp; """")</f>
-        <v>L["LogBook %s initialized"] = "LogBook %s inicializado"</v>
+        <v>L["Module |cffffcc00%s|r loaded"] = "Módulo |cffffcc00%s|r cargado"</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,11 +1076,11 @@
       </c>
       <c r="C24" s="1" t="str">
         <f aca="false">IF(A24="", "", "L["""&amp;A24&amp;"""] = true")</f>
-        <v>L["Left Click"] = true</v>
+        <v>L["LogBook %s initialized"] = true</v>
       </c>
       <c r="D24" s="1" t="str">
         <f aca="false">IF(A24="", "", "L["""&amp;A24&amp;"""] = """ &amp; B24 &amp; """")</f>
-        <v>L["Left Click"] = "Clic Izquierdo"</v>
+        <v>L["LogBook %s initialized"] = "LogBook %s inicializado"</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1017,11 +1092,11 @@
       </c>
       <c r="C25" s="1" t="str">
         <f aca="false">IF(A25="", "", "L["""&amp;A25&amp;"""] = true")</f>
-        <v>L["Open main window"] = true</v>
+        <v>L["Left Click"] = true</v>
       </c>
       <c r="D25" s="1" t="str">
         <f aca="false">IF(A25="", "", "L["""&amp;A25&amp;"""] = """ &amp; B25 &amp; """")</f>
-        <v>L["Open main window"] = "Abrir la ventana principal"</v>
+        <v>L["Left Click"] = "Clic Izquierdo"</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,11 +1108,11 @@
       </c>
       <c r="C26" s="1" t="str">
         <f aca="false">IF(A26="", "", "L["""&amp;A26&amp;"""] = true")</f>
-        <v>L["Right Click"] = true</v>
+        <v>L["Open main window"] = true</v>
       </c>
       <c r="D26" s="1" t="str">
         <f aca="false">IF(A26="", "", "L["""&amp;A26&amp;"""] = """ &amp; B26 &amp; """")</f>
-        <v>L["Right Click"] = "Clic Derecho"</v>
+        <v>L["Open main window"] = "Abrir la ventana principal"</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,11 +1124,11 @@
       </c>
       <c r="C27" s="1" t="str">
         <f aca="false">IF(A27="", "", "L["""&amp;A27&amp;"""] = true")</f>
-        <v>L["Open settings window"] = true</v>
+        <v>L["Right Click"] = true</v>
       </c>
       <c r="D27" s="1" t="str">
         <f aca="false">IF(A27="", "", "L["""&amp;A27&amp;"""] = """ &amp; B27 &amp; """")</f>
-        <v>L["Open settings window"] = "Abrir la ventana de configuración"</v>
+        <v>L["Right Click"] = "Clic Derecho"</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,11 +1140,11 @@
       </c>
       <c r="C28" s="1" t="str">
         <f aca="false">IF(A28="", "", "L["""&amp;A28&amp;"""] = true")</f>
-        <v>L["Advanced"] = true</v>
+        <v>L["Open settings window"] = true</v>
       </c>
       <c r="D28" s="1" t="str">
         <f aca="false">IF(A28="", "", "L["""&amp;A28&amp;"""] = """ &amp; B28 &amp; """")</f>
-        <v>L["Advanced"] = "Avanzado"</v>
+        <v>L["Open settings window"] = "Abrir la ventana de configuración"</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,11 +1156,11 @@
       </c>
       <c r="C29" s="1" t="str">
         <f aca="false">IF(A29="", "", "L["""&amp;A29&amp;"""] = true")</f>
-        <v>L["Advanced settings"] = true</v>
+        <v>L["Advanced"] = true</v>
       </c>
       <c r="D29" s="1" t="str">
         <f aca="false">IF(A29="", "", "L["""&amp;A29&amp;"""] = """ &amp; B29 &amp; """")</f>
-        <v>L["Advanced settings"] = "Ajustes avanzados"</v>
+        <v>L["Advanced"] = "Avanzado"</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,11 +1172,11 @@
       </c>
       <c r="C30" s="1" t="str">
         <f aca="false">IF(A30="", "", "L["""&amp;A30&amp;"""] = true")</f>
-        <v>L["Debug"] = true</v>
+        <v>L["Advanced settings"] = true</v>
       </c>
       <c r="D30" s="1" t="str">
         <f aca="false">IF(A30="", "", "L["""&amp;A30&amp;"""] = """ &amp; B30 &amp; """")</f>
-        <v>L["Debug"] = "Depurar"</v>
+        <v>L["Advanced settings"] = "Ajustes avanzados"</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,11 +1188,11 @@
       </c>
       <c r="C31" s="1" t="str">
         <f aca="false">IF(A31="", "", "L["""&amp;A31&amp;"""] = true")</f>
-        <v>L["Enable debug"] = true</v>
+        <v>L["Debug"] = true</v>
       </c>
       <c r="D31" s="1" t="str">
         <f aca="false">IF(A31="", "", "L["""&amp;A31&amp;"""] = """ &amp; B31 &amp; """")</f>
-        <v>L["Enable debug"] = "Habilitar depuración"</v>
+        <v>L["Debug"] = "Depurar"</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,31 +1200,31 @@
         <v>59</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C32" s="1" t="str">
         <f aca="false">IF(A32="", "", "L["""&amp;A32&amp;"""] = true")</f>
-        <v>L["General"] = true</v>
+        <v>L["Enable debug"] = true</v>
       </c>
       <c r="D32" s="1" t="str">
         <f aca="false">IF(A32="", "", "L["""&amp;A32&amp;"""] = """ &amp; B32 &amp; """")</f>
-        <v>L["General"] = "General"</v>
+        <v>L["Enable debug"] = "Habilitar depuración"</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C33" s="1" t="str">
         <f aca="false">IF(A33="", "", "L["""&amp;A33&amp;"""] = true")</f>
-        <v>L["General settings"] = true</v>
+        <v>L["General"] = true</v>
       </c>
       <c r="D33" s="1" t="str">
         <f aca="false">IF(A33="", "", "L["""&amp;A33&amp;"""] = """ &amp; B33 &amp; """")</f>
-        <v>L["General settings"] = "Configuración general"</v>
+        <v>L["General"] = "General"</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1161,11 +1236,11 @@
       </c>
       <c r="C34" s="1" t="str">
         <f aca="false">IF(A34="", "", "L["""&amp;A34&amp;"""] = true")</f>
-        <v>L["Log|cff57b6ffBook|r available commands"] = true</v>
+        <v>L["General settings"] = true</v>
       </c>
       <c r="D34" s="1" t="str">
         <f aca="false">IF(A34="", "", "L["""&amp;A34&amp;"""] = """ &amp; B34 &amp; """")</f>
-        <v>L["Log|cff57b6ffBook|r available commands"] = "Comandos disponibles de Log|cff57b6ffBook|r"</v>
+        <v>L["General settings"] = "Configuración general"</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1177,11 +1252,11 @@
       </c>
       <c r="C35" s="1" t="str">
         <f aca="false">IF(A35="", "", "L["""&amp;A35&amp;"""] = true")</f>
-        <v>L["Open critics window"] = true</v>
+        <v>L["Log|cff57b6ffBook|r available commands"] = true</v>
       </c>
       <c r="D35" s="1" t="str">
         <f aca="false">IF(A35="", "", "L["""&amp;A35&amp;"""] = """ &amp; B35 &amp; """")</f>
-        <v>L["Open critics window"] = "Abrir ventana de críticos"</v>
+        <v>L["Log|cff57b6ffBook|r available commands"] = "Comandos disponibles de Log|cff57b6ffBook|r"</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,11 +1268,11 @@
       </c>
       <c r="C36" s="1" t="str">
         <f aca="false">IF(A36="", "", "L["""&amp;A36&amp;"""] = true")</f>
-        <v>L["Open loot window"] = true</v>
+        <v>L["Open critics window"] = true</v>
       </c>
       <c r="D36" s="1" t="str">
         <f aca="false">IF(A36="", "", "L["""&amp;A36&amp;"""] = """ &amp; B36 &amp; """")</f>
-        <v>L["Open loot window"] = "Abrir ventana de botín"</v>
+        <v>L["Open critics window"] = "Abrir ventana de críticos"</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1209,11 +1284,11 @@
       </c>
       <c r="C37" s="1" t="str">
         <f aca="false">IF(A37="", "", "L["""&amp;A37&amp;"""] = true")</f>
-        <v>L["Open zones window"] = true</v>
+        <v>L["Open loot window"] = true</v>
       </c>
       <c r="D37" s="1" t="str">
         <f aca="false">IF(A37="", "", "L["""&amp;A37&amp;"""] = """ &amp; B37 &amp; """")</f>
-        <v>L["Open zones window"] = "Abrir la ventana de zonas"</v>
+        <v>L["Open loot window"] = "Abrir ventana de botín"</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1225,11 +1300,11 @@
       </c>
       <c r="C38" s="1" t="str">
         <f aca="false">IF(A38="", "", "L["""&amp;A38&amp;"""] = true")</f>
-        <v>L["Open fishing window"] = true</v>
+        <v>L["Open zones window"] = true</v>
       </c>
       <c r="D38" s="1" t="str">
         <f aca="false">IF(A38="", "", "L["""&amp;A38&amp;"""] = """ &amp; B38 &amp; """")</f>
-        <v>L["Open fishing window"] = "Abrir la ventana de pesca"</v>
+        <v>L["Open zones window"] = "Abrir la ventana de zonas"</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1241,11 +1316,11 @@
       </c>
       <c r="C39" s="1" t="str">
         <f aca="false">IF(A39="", "", "L["""&amp;A39&amp;"""] = true")</f>
-        <v>L["Open mobs window"] = true</v>
+        <v>L["Open fishing window"] = true</v>
       </c>
       <c r="D39" s="1" t="str">
         <f aca="false">IF(A39="", "", "L["""&amp;A39&amp;"""] = """ &amp; B39 &amp; """")</f>
-        <v>L["Open mobs window"] = "Abrir la ventana de mobs"</v>
+        <v>L["Open fishing window"] = "Abrir la ventana de pesca"</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1257,11 +1332,11 @@
       </c>
       <c r="C40" s="1" t="str">
         <f aca="false">IF(A40="", "", "L["""&amp;A40&amp;"""] = true")</f>
-        <v>L["Open enchanting window"] = true</v>
+        <v>L["Open mobs window"] = true</v>
       </c>
       <c r="D40" s="1" t="str">
         <f aca="false">IF(A40="", "", "L["""&amp;A40&amp;"""] = """ &amp; B40 &amp; """")</f>
-        <v>L["Open enchanting window"] = "Abrir la ventana de encantamiento"</v>
+        <v>L["Open mobs window"] = "Abrir la ventana de mobs"</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,11 +1348,11 @@
       </c>
       <c r="C41" s="1" t="str">
         <f aca="false">IF(A41="", "", "L["""&amp;A41&amp;"""] = true")</f>
-        <v>L["Main plugins"] = true</v>
+        <v>L["Open enchanting window"] = true</v>
       </c>
       <c r="D41" s="1" t="str">
         <f aca="false">IF(A41="", "", "L["""&amp;A41&amp;"""] = """ &amp; B41 &amp; """")</f>
-        <v>L["Main plugins"] = "Plugins principales"</v>
+        <v>L["Open enchanting window"] = "Abrir la ventana de encantamiento"</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1289,14 +1364,14 @@
       </c>
       <c r="C42" s="1" t="str">
         <f aca="false">IF(A42="", "", "L["""&amp;A42&amp;"""] = true")</f>
-        <v>L["Loot"] = true</v>
+        <v>L["Main plugins"] = true</v>
       </c>
       <c r="D42" s="1" t="str">
         <f aca="false">IF(A42="", "", "L["""&amp;A42&amp;"""] = """ &amp; B42 &amp; """")</f>
-        <v>L["Loot"] = "Botín"</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Main plugins"] = "Plugins principales"</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>80</v>
       </c>
@@ -1305,14 +1380,14 @@
       </c>
       <c r="C43" s="1" t="str">
         <f aca="false">IF(A43="", "", "L["""&amp;A43&amp;"""] = true")</f>
-        <v>L["Allows you to track loot and items crafted with trading skills."] = true</v>
+        <v>L["Loot"] = true</v>
       </c>
       <c r="D43" s="1" t="str">
         <f aca="false">IF(A43="", "", "L["""&amp;A43&amp;"""] = """ &amp; B43 &amp; """")</f>
-        <v>L["Allows you to track loot and items crafted with trading skills."] = "Permite realizar un seguimiento del botín y los artículos elaborados con habilidades comerciales."</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Loot"] = "Botín"</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>82</v>
       </c>
@@ -1321,14 +1396,14 @@
       </c>
       <c r="C44" s="1" t="str">
         <f aca="false">IF(A44="", "", "L["""&amp;A44&amp;"""] = true")</f>
-        <v>L["Fishing"] = true</v>
+        <v>L["Allows you to track loot and items crafted with trading skills."] = true</v>
       </c>
       <c r="D44" s="1" t="str">
         <f aca="false">IF(A44="", "", "L["""&amp;A44&amp;"""] = """ &amp; B44 &amp; """")</f>
-        <v>L["Fishing"] = "Pesca"</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Allows you to track loot and items crafted with trading skills."] = "Permite realizar un seguimiento del botín y los artículos elaborados con habilidades comerciales."</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
         <v>84</v>
       </c>
@@ -1337,14 +1412,14 @@
       </c>
       <c r="C45" s="1" t="str">
         <f aca="false">IF(A45="", "", "L["""&amp;A45&amp;"""] = true")</f>
-        <v>L["Allows you to track fish from pools and wreckages."] = true</v>
+        <v>L["Fishing"] = true</v>
       </c>
       <c r="D45" s="1" t="str">
         <f aca="false">IF(A45="", "", "L["""&amp;A45&amp;"""] = """ &amp; B45 &amp; """")</f>
-        <v>L["Allows you to track fish from pools and wreckages."] = "Permite realizar un seguimiento de peces desde pozas y restos de naufragios."</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Fishing"] = "Pesca"</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
         <v>86</v>
       </c>
@@ -1353,14 +1428,14 @@
       </c>
       <c r="C46" s="1" t="str">
         <f aca="false">IF(A46="", "", "L["""&amp;A46&amp;"""] = true")</f>
-        <v>L["Critics"] = true</v>
+        <v>L["Allows you to track fish from pools and wreckages."] = true</v>
       </c>
       <c r="D46" s="1" t="str">
         <f aca="false">IF(A46="", "", "L["""&amp;A46&amp;"""] = """ &amp; B46 &amp; """")</f>
-        <v>L["Critics"] = "Críticos"</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Allows you to track fish from pools and wreckages."] = "Permite realizar un seguimiento de peces desde pozas y restos de naufragios."</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>88</v>
       </c>
@@ -1369,14 +1444,14 @@
       </c>
       <c r="C47" s="1" t="str">
         <f aca="false">IF(A47="", "", "L["""&amp;A47&amp;"""] = true")</f>
-        <v>L["Allows you to track hits or healing, both normal and critical."] = true</v>
+        <v>L["Critics"] = true</v>
       </c>
       <c r="D47" s="1" t="str">
         <f aca="false">IF(A47="", "", "L["""&amp;A47&amp;"""] = """ &amp; B47 &amp; """")</f>
-        <v>L["Allows you to track hits or healing, both normal and critical."] = "Permite realizar un seguimiento de los golpes o curaciones, tanto normales como críticos."</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Critics"] = "Críticos"</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
         <v>90</v>
       </c>
@@ -1385,11 +1460,11 @@
       </c>
       <c r="C48" s="1" t="str">
         <f aca="false">IF(A48="", "", "L["""&amp;A48&amp;"""] = true")</f>
-        <v>L["Zones"] = true</v>
+        <v>L["Allows you to track hits or healing, both normal and critical."] = true</v>
       </c>
       <c r="D48" s="1" t="str">
         <f aca="false">IF(A48="", "", "L["""&amp;A48&amp;"""] = """ &amp; B48 &amp; """")</f>
-        <v>L["Zones"] = "Zonas"</v>
+        <v>L["Allows you to track hits or healing, both normal and critical."] = "Permite realizar un seguimiento de los golpes o curaciones, tanto normales como críticos."</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,11 +1476,11 @@
       </c>
       <c r="C49" s="1" t="str">
         <f aca="false">IF(A49="", "", "L["""&amp;A49&amp;"""] = true")</f>
-        <v>L["Allows you to track zones."] = true</v>
+        <v>L["Zones"] = true</v>
       </c>
       <c r="D49" s="1" t="str">
         <f aca="false">IF(A49="", "", "L["""&amp;A49&amp;"""] = """ &amp; B49 &amp; """")</f>
-        <v>L["Allows you to track zones."] = "Permite realizar un seguimiento de las zonas."</v>
+        <v>L["Zones"] = "Zonas"</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1413,31 +1488,31 @@
         <v>94</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C50" s="1" t="str">
         <f aca="false">IF(A50="", "", "L["""&amp;A50&amp;"""] = true")</f>
-        <v>L["Mobs"] = true</v>
+        <v>L["Allows you to track zones."] = true</v>
       </c>
       <c r="D50" s="1" t="str">
         <f aca="false">IF(A50="", "", "L["""&amp;A50&amp;"""] = """ &amp; B50 &amp; """")</f>
-        <v>L["Mobs"] = "Mobs"</v>
+        <v>L["Allows you to track zones."] = "Permite realizar un seguimiento de las zonas."</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>96</v>
       </c>
       <c r="C51" s="1" t="str">
         <f aca="false">IF(A51="", "", "L["""&amp;A51&amp;"""] = true")</f>
-        <v>L["Allows you to track mobs."] = true</v>
+        <v>L["Mobs"] = true</v>
       </c>
       <c r="D51" s="1" t="str">
         <f aca="false">IF(A51="", "", "L["""&amp;A51&amp;"""] = """ &amp; B51 &amp; """")</f>
-        <v>L["Allows you to track mobs."] = "Permite realizar un seguimiento de las mobs."</v>
+        <v>L["Mobs"] = "Mobs"</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1449,11 +1524,11 @@
       </c>
       <c r="C52" s="1" t="str">
         <f aca="false">IF(A52="", "", "L["""&amp;A52&amp;"""] = true")</f>
-        <v>L["Enchanting"] = true</v>
+        <v>L["Allows you to track mobs."] = true</v>
       </c>
       <c r="D52" s="1" t="str">
         <f aca="false">IF(A52="", "", "L["""&amp;A52&amp;"""] = """ &amp; B52 &amp; """")</f>
-        <v>L["Enchanting"] = "Encantamiento"</v>
+        <v>L["Allows you to track mobs."] = "Permite realizar un seguimiento de las mobs."</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,11 +1540,11 @@
       </c>
       <c r="C53" s="1" t="str">
         <f aca="false">IF(A53="", "", "L["""&amp;A53&amp;"""] = true")</f>
-        <v>L["Allows you to track enchanting."] = true</v>
+        <v>L["Enchanting"] = true</v>
       </c>
       <c r="D53" s="1" t="str">
         <f aca="false">IF(A53="", "", "L["""&amp;A53&amp;"""] = """ &amp; B53 &amp; """")</f>
-        <v>L["Allows you to track enchanting."] = "Permite realizar un seguimiento de encantamiento."</v>
+        <v>L["Enchanting"] = "Encantamiento"</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,11 +1556,11 @@
       </c>
       <c r="C54" s="1" t="str">
         <f aca="false">IF(A54="", "", "L["""&amp;A54&amp;"""] = true")</f>
-        <v>L["Settings"] = true</v>
+        <v>L["Allows you to track enchanting."] = true</v>
       </c>
       <c r="D54" s="1" t="str">
         <f aca="false">IF(A54="", "", "L["""&amp;A54&amp;"""] = """ &amp; B54 &amp; """")</f>
-        <v>L["Settings"] = "Configuración"</v>
+        <v>L["Allows you to track enchanting."] = "Permite realizar un seguimiento de encantamiento."</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,11 +1572,11 @@
       </c>
       <c r="C55" s="1" t="str">
         <f aca="false">IF(A55="", "", "L["""&amp;A55&amp;"""] = true")</f>
-        <v>L["Stats"] = true</v>
+        <v>L["Settings"] = true</v>
       </c>
       <c r="D55" s="1" t="str">
         <f aca="false">IF(A55="", "", "L["""&amp;A55&amp;"""] = """ &amp; B55 &amp; """")</f>
-        <v>L["Stats"] = "Estadísticas"</v>
+        <v>L["Settings"] = "Configuración"</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1513,14 +1588,14 @@
       </c>
       <c r="C56" s="1" t="str">
         <f aca="false">IF(A56="", "", "L["""&amp;A56&amp;"""] = true")</f>
-        <v>L["Maintenance"] = true</v>
+        <v>L["Stats"] = true</v>
       </c>
       <c r="D56" s="1" t="str">
         <f aca="false">IF(A56="", "", "L["""&amp;A56&amp;"""] = """ &amp; B56 &amp; """")</f>
-        <v>L["Maintenance"] = "Mantenimiento"</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Stats"] = "Estadísticas"</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>107</v>
       </c>
@@ -1529,14 +1604,14 @@
       </c>
       <c r="C57" s="1" t="str">
         <f aca="false">IF(A57="", "", "L["""&amp;A57&amp;"""] = true")</f>
-        <v>L["Starting database auto update: %s"] = true</v>
+        <v>L["Tooltips"] = true</v>
       </c>
       <c r="D57" s="1" t="str">
         <f aca="false">IF(A57="", "", "L["""&amp;A57&amp;"""] = """ &amp; B57 &amp; """")</f>
-        <v>L["Starting database auto update: %s"] = "Iniciando la actualización automática de la base de datos: %s"</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Tooltips"] = "Mensaje emergente"</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
         <v>109</v>
       </c>
@@ -1545,14 +1620,14 @@
       </c>
       <c r="C58" s="1" t="str">
         <f aca="false">IF(A58="", "", "L["""&amp;A58&amp;"""] = true")</f>
-        <v>L["Cancelling database auto update: %s"] = true</v>
+        <v>L["Maintenance"] = true</v>
       </c>
       <c r="D58" s="1" t="str">
         <f aca="false">IF(A58="", "", "L["""&amp;A58&amp;"""] = """ &amp; B58 &amp; """")</f>
-        <v>L["Cancelling database auto update: %s"] = "Cancelando la actualización automática de la base de datos: %s"</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Maintenance"] = "Mantenimiento"</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
         <v>111</v>
       </c>
@@ -1561,14 +1636,14 @@
       </c>
       <c r="C59" s="1" t="str">
         <f aca="false">IF(A59="", "", "L["""&amp;A59&amp;"""] = true")</f>
-        <v>L["%s database update: %s"] = true</v>
+        <v>L["Starting database auto update: %s"] = true</v>
       </c>
       <c r="D59" s="1" t="str">
         <f aca="false">IF(A59="", "", "L["""&amp;A59&amp;"""] = """ &amp; B59 &amp; """")</f>
-        <v>L["%s database update: %s"] = "Actualización base de datos %s : %s"</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>L["Starting database auto update: %s"] = "Iniciando la actualización automática de la base de datos: %s"</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
         <v>113</v>
       </c>
@@ -1577,11 +1652,11 @@
       </c>
       <c r="C60" s="1" t="str">
         <f aca="false">IF(A60="", "", "L["""&amp;A60&amp;"""] = true")</f>
-        <v>L["Done!"] = true</v>
+        <v>L["Cancelling database auto update: %s"] = true</v>
       </c>
       <c r="D60" s="1" t="str">
         <f aca="false">IF(A60="", "", "L["""&amp;A60&amp;"""] = """ &amp; B60 &amp; """")</f>
-        <v>L["Done!"] = "¡Hecho!"</v>
+        <v>L["Cancelling database auto update: %s"] = "Cancelando la actualización automática de la base de datos: %s"</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,11 +1668,11 @@
       </c>
       <c r="C61" s="1" t="str">
         <f aca="false">IF(A61="", "", "L["""&amp;A61&amp;"""] = true")</f>
-        <v>L["Tooltips"] = true</v>
+        <v>L["%s database update: %s"] = true</v>
       </c>
       <c r="D61" s="1" t="str">
         <f aca="false">IF(A61="", "", "L["""&amp;A61&amp;"""] = """ &amp; B61 &amp; """")</f>
-        <v>L["Tooltips"] = "Mensaje emergente"</v>
+        <v>L["%s database update: %s"] = "Actualización base de datos %s : %s"</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1609,11 +1684,11 @@
       </c>
       <c r="C62" s="1" t="str">
         <f aca="false">IF(A62="", "", "L["""&amp;A62&amp;"""] = true")</f>
-        <v>L["Database"] = true</v>
+        <v>L["Done!"] = true</v>
       </c>
       <c r="D62" s="1" t="str">
         <f aca="false">IF(A62="", "", "L["""&amp;A62&amp;"""] = """ &amp; B62 &amp; """")</f>
-        <v>L["Database"] = "Base de datos"</v>
+        <v>L["Done!"] = "¡Hecho!"</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,11 +1700,11 @@
       </c>
       <c r="C63" s="1" t="str">
         <f aca="false">IF(A63="", "", "L["""&amp;A63&amp;"""] = true")</f>
-        <v>L["Press key to show"] = true</v>
+        <v>L["All"] = true</v>
       </c>
       <c r="D63" s="1" t="str">
         <f aca="false">IF(A63="", "", "L["""&amp;A63&amp;"""] = """ &amp; B63 &amp; """")</f>
-        <v>L["Press key to show"] = "Pulse la tecla para mostrar"</v>
+        <v>L["All"] = "Todos"</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1641,11 +1716,11 @@
       </c>
       <c r="C64" s="1" t="str">
         <f aca="false">IF(A64="", "", "L["""&amp;A64&amp;"""] = true")</f>
-        <v>L["more"] = true</v>
+        <v>L["Database"] = true</v>
       </c>
       <c r="D64" s="1" t="str">
         <f aca="false">IF(A64="", "", "L["""&amp;A64&amp;"""] = """ &amp; B64 &amp; """")</f>
-        <v>L["more"] = "más"</v>
+        <v>L["Database"] = "Base de datos"</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1657,11 +1732,11 @@
       </c>
       <c r="C65" s="1" t="str">
         <f aca="false">IF(A65="", "", "L["""&amp;A65&amp;"""] = true")</f>
-        <v>L["Character"] = true</v>
+        <v>L["more"] = true</v>
       </c>
       <c r="D65" s="1" t="str">
         <f aca="false">IF(A65="", "", "L["""&amp;A65&amp;"""] = """ &amp; B65 &amp; """")</f>
-        <v>L["Character"] = "Personaje"</v>
+        <v>L["more"] = "más"</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1669,145 +1744,223 @@
         <v>125</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C66" s="1" t="str">
         <f aca="false">IF(A66="", "", "L["""&amp;A66&amp;"""] = true")</f>
-        <v>L["Character name."] = true</v>
+        <v>L["Normal"] = true</v>
       </c>
       <c r="D66" s="1" t="str">
         <f aca="false">IF(A66="", "", "L["""&amp;A66&amp;"""] = """ &amp; B66 &amp; """")</f>
-        <v>L["Character name."] = "Nombre del personaje."</v>
+        <v>L["Normal"] = "Normal"</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="C67" s="1" t="str">
         <f aca="false">IF(A67="", "", "L["""&amp;A67&amp;"""] = true")</f>
-        <v/>
+        <v>L["Rare"] = true</v>
       </c>
       <c r="D67" s="1" t="str">
         <f aca="false">IF(A67="", "", "L["""&amp;A67&amp;"""] = """ &amp; B67 &amp; """")</f>
-        <v/>
+        <v>L["Rare"] = "Raro"</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="C68" s="1" t="str">
         <f aca="false">IF(A68="", "", "L["""&amp;A68&amp;"""] = true")</f>
-        <v/>
+        <v>L["Elite"] = true</v>
       </c>
       <c r="D68" s="1" t="str">
         <f aca="false">IF(A68="", "", "L["""&amp;A68&amp;"""] = """ &amp; B68 &amp; """")</f>
-        <v/>
+        <v>L["Elite"] = "Élite"</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="C69" s="1" t="str">
         <f aca="false">IF(A69="", "", "L["""&amp;A69&amp;"""] = true")</f>
-        <v/>
+        <v>L["Rare elite"] = true</v>
       </c>
       <c r="D69" s="1" t="str">
         <f aca="false">IF(A69="", "", "L["""&amp;A69&amp;"""] = """ &amp; B69 &amp; """")</f>
-        <v/>
+        <v>L["Rare elite"] = "Raro élite"</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="C70" s="1" t="str">
         <f aca="false">IF(A70="", "", "L["""&amp;A70&amp;"""] = true")</f>
-        <v/>
+        <v>L["Boss"] = true</v>
       </c>
       <c r="D70" s="1" t="str">
         <f aca="false">IF(A70="", "", "L["""&amp;A70&amp;"""] = """ &amp; B70 &amp; """")</f>
-        <v/>
+        <v>L["Boss"] = "Jefe"</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="C71" s="1" t="str">
         <f aca="false">IF(A71="", "", "L["""&amp;A71&amp;"""] = true")</f>
-        <v/>
+        <v>L["World boss"] = true</v>
       </c>
       <c r="D71" s="1" t="str">
         <f aca="false">IF(A71="", "", "L["""&amp;A71&amp;"""] = """ &amp; B71 &amp; """")</f>
-        <v/>
+        <v>L["World boss"] = "Jefe de mundo"</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="C72" s="1" t="str">
         <f aca="false">IF(A72="", "", "L["""&amp;A72&amp;"""] = true")</f>
-        <v/>
+        <v>L["Poor"] = true</v>
       </c>
       <c r="D72" s="1" t="str">
         <f aca="false">IF(A72="", "", "L["""&amp;A72&amp;"""] = """ &amp; B72 &amp; """")</f>
-        <v/>
+        <v>L["Poor"] = "Pobre"</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="C73" s="1" t="str">
         <f aca="false">IF(A73="", "", "L["""&amp;A73&amp;"""] = true")</f>
-        <v/>
+        <v>L["Common"] = true</v>
       </c>
       <c r="D73" s="1" t="str">
         <f aca="false">IF(A73="", "", "L["""&amp;A73&amp;"""] = """ &amp; B73 &amp; """")</f>
-        <v/>
+        <v>L["Common"] = "Común"</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="C74" s="1" t="str">
         <f aca="false">IF(A74="", "", "L["""&amp;A74&amp;"""] = true")</f>
-        <v/>
+        <v>L["Uncommon"] = true</v>
       </c>
       <c r="D74" s="1" t="str">
         <f aca="false">IF(A74="", "", "L["""&amp;A74&amp;"""] = """ &amp; B74 &amp; """")</f>
-        <v/>
+        <v>L["Uncommon"] = "Poco Común"</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="C75" s="1" t="str">
         <f aca="false">IF(A75="", "", "L["""&amp;A75&amp;"""] = true")</f>
-        <v/>
+        <v>L["Epic"] = true</v>
       </c>
       <c r="D75" s="1" t="str">
         <f aca="false">IF(A75="", "", "L["""&amp;A75&amp;"""] = """ &amp; B75 &amp; """")</f>
-        <v/>
+        <v>L["Epic"] = "Epico"</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="C76" s="1" t="str">
         <f aca="false">IF(A76="", "", "L["""&amp;A76&amp;"""] = true")</f>
-        <v/>
+        <v>L["Legendary"] = true</v>
       </c>
       <c r="D76" s="1" t="str">
         <f aca="false">IF(A76="", "", "L["""&amp;A76&amp;"""] = """ &amp; B76 &amp; """")</f>
-        <v/>
+        <v>L["Legendary"] = "Legendario"</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="C77" s="1" t="str">
         <f aca="false">IF(A77="", "", "L["""&amp;A77&amp;"""] = true")</f>
-        <v/>
+        <v>L["Artifact"] = true</v>
       </c>
       <c r="D77" s="1" t="str">
         <f aca="false">IF(A77="", "", "L["""&amp;A77&amp;"""] = """ &amp; B77 &amp; """")</f>
-        <v/>
+        <v>L["Artifact"] = "Artefacto"</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="C78" s="1" t="str">
         <f aca="false">IF(A78="", "", "L["""&amp;A78&amp;"""] = true")</f>
-        <v/>
+        <v>L["Heirloom"] = true</v>
       </c>
       <c r="D78" s="1" t="str">
         <f aca="false">IF(A78="", "", "L["""&amp;A78&amp;"""] = """ &amp; B78 &amp; """")</f>
-        <v/>
+        <v>L["Heirloom"] = "Reliquia"</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="C79" s="1" t="str">
         <f aca="false">IF(A79="", "", "L["""&amp;A79&amp;"""] = true")</f>
-        <v/>
+        <v>L["WoW Token"] = true</v>
       </c>
       <c r="D79" s="1" t="str">
         <f aca="false">IF(A79="", "", "L["""&amp;A79&amp;"""] = """ &amp; B79 &amp; """")</f>
-        <v/>
+        <v>L["WoW Token"] = "Ficha WoW"</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>